<commit_message>
Update template excel document
</commit_message>
<xml_diff>
--- a/TECNM.Residencias/Resources/TemplateDocument.xlsx
+++ b/TECNM.Residencias/Resources/TemplateDocument.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD5646E-9825-47A2-B5AF-8B18E3E21201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E699ADB2-A022-4C45-A526-2D3FC6ADFB6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2C1378D0-2801-4854-B5EC-4FF10D8C49AF}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId9"/>
     <pivotCache cacheId="1" r:id="rId10"/>
-    <pivotCache cacheId="6" r:id="rId11"/>
+    <pivotCache cacheId="2" r:id="rId11"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="21">
   <si>
     <t>Nombre</t>
   </si>
@@ -102,13 +102,10 @@
     <t>Tipo</t>
   </si>
   <si>
-    <t>Etiquetas de fila</t>
+    <t>Habiliad</t>
   </si>
   <si>
-    <t>Cuenta de Tipo</t>
-  </si>
-  <si>
-    <t>Cuenta de Habilidad</t>
+    <t>Conteo</t>
   </si>
 </sst>
 </file>
@@ -150,10 +147,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9387,22 +9384,22 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{360BCCA9-0BC8-48FA-858C-577346306641}" name="TablaDinámica1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="E1:G4" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{360BCCA9-0BC8-48FA-858C-577346306641}" name="TablaDinámica1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Habiliad">
+  <location ref="E1:F4" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
-    <pivotField axis="axisRow" dataField="1" showAll="0">
+    <pivotField axis="axisRow" showAll="0">
       <items count="2">
         <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
+    <pivotField axis="axisRow" showAll="0">
       <items count="2">
         <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
   </pivotFields>
   <rowFields count="2">
     <field x="1"/>
@@ -9419,20 +9416,11 @@
       <x/>
     </i>
   </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
+  <colItems count="1">
+    <i/>
   </colItems>
-  <dataFields count="2">
-    <dataField name="Cuenta de Tipo" fld="1" subtotal="count" baseField="0" baseItem="0"/>
-    <dataField name="Cuenta de Habilidad" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  <dataFields count="1">
+    <dataField name="Conteo" fld="2" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -9447,80 +9435,6 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{375901E5-9438-4C85-9538-66D8BB885B6C}" name="TablaDinámica5" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5" rowHeaderCaption="Expediente cerrado">
-  <location ref="L20:M22" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="12">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="2">
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="11"/>
-  </rowFields>
-  <rowItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Total" fld="11" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="2">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="2">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="11" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{54AC48D3-112B-4403-877C-49444D3B1092}" name="TablaDinámica4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="Semestre">
   <location ref="L1:M3" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
@@ -9594,7 +9508,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E012B798-023A-429E-B0F5-1F3284F84ED5}" name="TablaDinámica3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="Género">
   <location ref="A20:B22" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
@@ -9668,7 +9582,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C32D114E-82DC-435A-B854-C94228D02013}" name="TablaDinámica2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" rowHeaderCaption="Especialidad">
   <location ref="A1:B3" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
@@ -9712,6 +9626,80 @@
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{375901E5-9438-4C85-9538-66D8BB885B6C}" name="TablaDinámica5" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5" rowHeaderCaption="Expediente cerrado">
+  <location ref="L20:M22" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="12">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="11"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Total" fld="11" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="2">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="11" count="1" selected="0">
             <x v="0"/>
           </reference>
         </references>
@@ -10412,7 +10400,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DC5092C-6A5D-4922-B145-77E669324C72}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -10420,11 +10408,11 @@
   <cols>
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -10440,30 +10428,24 @@
       <c r="F1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
-        <v>21</v>
-      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E3" s="4" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="F4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update excel template file
</commit_message>
<xml_diff>
--- a/TECNM.Residencias/Resources/TemplateDocument.xlsx
+++ b/TECNM.Residencias/Resources/TemplateDocument.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E699ADB2-A022-4C45-A526-2D3FC6ADFB6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C6FA2AC-1C63-414F-82EF-89D227CC3A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2C1378D0-2801-4854-B5EC-4FF10D8C49AF}"/>
   </bookViews>
@@ -141,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -150,7 +150,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -193,9 +192,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
+                  <a:schemeClr val="dk1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
@@ -225,9 +224,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="dk1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
@@ -249,15 +248,20 @@
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
-          <a:ln w="19050">
-            <a:solidFill>
-              <a:schemeClr val="lt1"/>
-            </a:solidFill>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="25000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
         </c:spPr>
         <c:marker>
-          <c:symbol val="none"/>
+          <c:symbol val="circle"/>
+          <c:size val="6"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -275,12 +279,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="lt1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -290,11 +291,12 @@
               <a:endParaRPr lang="es-MX"/>
             </a:p>
           </c:txPr>
+          <c:dLblPos val="inEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
+          <c:showPercent val="1"/>
           <c:showBubbleSize val="0"/>
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
@@ -307,12 +309,16 @@
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
-          <a:ln w="19050">
-            <a:solidFill>
-              <a:schemeClr val="lt1"/>
-            </a:solidFill>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="25000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
         </c:spPr>
       </c:pivotFmt>
     </c:pivotFmts>
@@ -341,12 +347,16 @@
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -354,6 +364,59 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Empresas!$E$2:$E$3</c:f>
@@ -381,11 +444,12 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="inEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
+          <c:showPercent val="1"/>
           <c:showBubbleSize val="0"/>
           <c:showLeaderLines val="1"/>
         </c:dLbls>
@@ -403,7 +467,11 @@
       <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
-        <a:noFill/>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="78000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -416,7 +484,7 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="dk1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
@@ -442,12 +510,19 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
+    <a:pattFill prst="dkDnDiag">
+      <a:fgClr>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
+      </a:fgClr>
+      <a:bgClr>
+        <a:schemeClr val="lt1"/>
+      </a:bgClr>
+    </a:pattFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
+        <a:schemeClr val="dk1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -4118,78 +4193,8 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="261">
   <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -4199,11 +4204,76 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="dkDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="lt1">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:ln>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="dk1">
             <a:lumMod val="25000"/>
@@ -4219,36 +4289,51 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="25000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="25400">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="88900" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="threePt" dir="t"/>
+      </a:scene3d>
+      <a:sp3d prstMaterial="matte"/>
     </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
@@ -4258,7 +4343,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="28575" cap="rnd">
@@ -4270,25 +4355,26 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="lt1"/>
         </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -4296,7 +4382,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -4312,7 +4398,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -4321,7 +4407,7 @@
       <a:noFill/>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -4336,7 +4422,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -4347,7 +4433,7 @@
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
@@ -4361,12 +4447,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
@@ -4380,12 +4466,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
@@ -4399,7 +4485,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:noFill/>
@@ -4413,12 +4499,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -4432,12 +4518,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
@@ -4451,12 +4537,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="50000"/>
             <a:lumOff val="50000"/>
           </a:schemeClr>
@@ -4470,12 +4556,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
@@ -4489,11 +4575,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:alpha val="78000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
   <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
@@ -4501,7 +4594,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
@@ -4509,7 +4602,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -4517,7 +4610,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -4529,12 +4622,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
@@ -4548,12 +4641,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -4562,14 +4655,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -4578,7 +4671,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -4590,7 +4683,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -4598,7 +4691,7 @@
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
@@ -4612,7 +4705,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -4624,14 +4717,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -9259,7 +9346,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9752B337-64DE-4187-9A60-317273E19197}" name="TablaDinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" rowHeaderCaption="Sector">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9752B337-64DE-4187-9A60-317273E19197}" name="TablaDinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="Sector">
   <location ref="E1:F3" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -9435,80 +9522,6 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{54AC48D3-112B-4403-877C-49444D3B1092}" name="TablaDinámica4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="Semestre">
-  <location ref="L1:M3" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="12">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="2">
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Total" fld="3" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="2">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="2">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E012B798-023A-429E-B0F5-1F3284F84ED5}" name="TablaDinámica3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="Género">
   <location ref="A20:B22" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
@@ -9582,7 +9595,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C32D114E-82DC-435A-B854-C94228D02013}" name="TablaDinámica2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" rowHeaderCaption="Especialidad">
   <location ref="A1:B3" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
@@ -9644,7 +9657,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{375901E5-9438-4C85-9538-66D8BB885B6C}" name="TablaDinámica5" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5" rowHeaderCaption="Expediente cerrado">
   <location ref="L20:M22" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
@@ -9700,6 +9713,80 @@
             <x v="0"/>
           </reference>
           <reference field="11" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{54AC48D3-112B-4403-877C-49444D3B1092}" name="TablaDinámica4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="Semestre">
+  <location ref="L1:M3" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="12">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Total" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="2">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
             <x v="0"/>
           </reference>
         </references>
@@ -10433,19 +10520,16 @@
       <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>